<commit_message>
Upload Project.doc Upload srs_trivia_rev_1_1.doc Updated CurrentSubmission.xlsx
</commit_message>
<xml_diff>
--- a/CurrentSubmission.xlsx
+++ b/CurrentSubmission.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\NWTC\NWTC School 3rd\Team Software Dev\Learning Plan 1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="220" yWindow="220" windowWidth="21360" windowHeight="19560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,11 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Current Submission for Team _________________________________</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Submission</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -41,30 +42,70 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>TurnIn1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test cases, SRS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test cases initial version
-SRS - Revised use cases and NF requirements</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <r>
+      <t>Current Submission for Team ___</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>Organization of Programming Students, OPS</t>
+    </r>
+  </si>
+  <si>
+    <t>ActDue01</t>
+  </si>
+  <si>
+    <t>Team Project Ideas</t>
+  </si>
+  <si>
+    <t>Team formation, proposed projects, summary of work to be done.</t>
+  </si>
+  <si>
+    <t>ActDue02</t>
+  </si>
+  <si>
+    <t>ActDue03</t>
+  </si>
+  <si>
+    <t>ActDue04</t>
+  </si>
+  <si>
+    <t>ActDue05</t>
+  </si>
+  <si>
+    <t>Software Selection</t>
+  </si>
+  <si>
+    <t>Software Requirements</t>
+  </si>
+  <si>
+    <t>Software Requirements Specification - Use cases division</t>
+  </si>
+  <si>
+    <t>Finshed SRS and posted</t>
+  </si>
+  <si>
+    <t>Finished SRS and posted to the BlackBoard</t>
+  </si>
+  <si>
+    <t>Selected Java and started creating the project classes and screens</t>
+  </si>
+  <si>
+    <t>First Sprint Started</t>
+  </si>
+  <si>
+    <t>Programminng Frames : Eric(SetupSummary), Ruth (AnswerEntry), Brian (QuestionSelect), Laercio (GameStatus) and Alesander (WinnerSelect)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -77,6 +118,17 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,12 +166,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -129,6 +186,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -451,185 +516,216 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
+    <col min="4" max="4" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="62" customHeight="1">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="4">
-        <v>38870</v>
-      </c>
-      <c r="C4" s="2" t="s">
+        <v>40789</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="62" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="62" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="62" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="62" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="62" customHeight="1">
-      <c r="A9" s="3"/>
+    <row r="5" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>40810</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>40817</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>40824</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4">
+        <v>40831</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
       <c r="B9" s="3"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:5" ht="62" customHeight="1">
+    <row r="10" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="62" customHeight="1">
+    <row r="11" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="62" customHeight="1">
+    <row r="12" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="62" customHeight="1">
+    <row r="13" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="62" customHeight="1">
+    <row r="14" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="62" customHeight="1">
+    <row r="15" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="62" customHeight="1">
+    <row r="16" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="62" customHeight="1">
+    <row r="17" spans="1:4" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="62" customHeight="1">
+    <row r="18" spans="1:4" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="62" customHeight="1">
+    <row r="19" spans="1:4" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="62" customHeight="1">
+    <row r="20" spans="1:4" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" ht="62" customHeight="1">
+    <row r="21" spans="1:4" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="62" customHeight="1">
+    <row r="22" spans="1:4" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" ht="62" customHeight="1">
+    <row r="23" spans="1:4" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" ht="62" customHeight="1">
+    <row r="24" spans="1:4" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" ht="62" customHeight="1">
+    <row r="25" spans="1:4" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>

</xml_diff>